<commit_message>
fix(backend): Arreglado un problema donde fallaba la importación de áreas debido a que se utilizaban ids incorrectos. Ahora las áreas permiten configurar sus siglas.
</commit_message>
<xml_diff>
--- a/tests/TestFiles/prueba_padron.xlsx
+++ b/tests/TestFiles/prueba_padron.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberto\Documents\proyectos\votacion-incubunt\tests\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4201399-3EB5-42B0-B84B-62A27B15B6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A711D-501E-44B2-9FDE-C2214F6433B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="192">
   <si>
     <t>diegoagreda51@gmail.com</t>
   </si>
@@ -189,33 +192,6 @@
     <t xml:space="preserve">Chávez Villanueva </t>
   </si>
   <si>
-    <t>echevarriapoemape@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">María De Los Ángeles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Echevarría Poémape </t>
-  </si>
-  <si>
-    <t>ya76larcat@gmail.com</t>
-  </si>
-  <si>
-    <t>Yamille del Pilar</t>
-  </si>
-  <si>
-    <t>Catacora Pinco</t>
-  </si>
-  <si>
-    <t>mellascon29@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mell Julia Kristell </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ascón Aranda </t>
-  </si>
-  <si>
     <t>lrosasp@unitru.edu.pe</t>
   </si>
   <si>
@@ -261,51 +237,6 @@
     <t>Acuña Cisneros</t>
   </si>
   <si>
-    <t>cerquinclaudia669@gmail.com</t>
-  </si>
-  <si>
-    <t>Claudia Yanela</t>
-  </si>
-  <si>
-    <t>Cerquín Alcántara</t>
-  </si>
-  <si>
-    <t>dlazaro@unitru.edu.pe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diana Carolina </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lázaro Solano </t>
-  </si>
-  <si>
-    <t>maria11.07.mfhs@gmail.com</t>
-  </si>
-  <si>
-    <t>Maria Fernanda</t>
-  </si>
-  <si>
-    <t>Holguin Solorzano</t>
-  </si>
-  <si>
-    <t>aurora_merlo@hotmail.com</t>
-  </si>
-  <si>
-    <t>Aurora Nicole</t>
-  </si>
-  <si>
-    <t>Merlo López</t>
-  </si>
-  <si>
-    <t>jcarlosquerebalu@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segundo Jeampier </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carlos Querebalú </t>
-  </si>
-  <si>
     <t>cbarretob@unitru.edu.pe</t>
   </si>
   <si>
@@ -396,15 +327,6 @@
     <t>Correa Urdániga</t>
   </si>
   <si>
-    <t>benitescasanovac@gmail.com</t>
-  </si>
-  <si>
-    <t>Chris Alexandra</t>
-  </si>
-  <si>
-    <t>Benites Casanova</t>
-  </si>
-  <si>
     <t>yasumi.2002.octubre@gmail.com</t>
   </si>
   <si>
@@ -603,15 +525,6 @@
     <t>Vizconde Julca</t>
   </si>
   <si>
-    <t>cristianparimango@gmail.com</t>
-  </si>
-  <si>
-    <t>Cristian Martín</t>
-  </si>
-  <si>
-    <t>Parimango Quispe</t>
-  </si>
-  <si>
     <t>e6666278@gmail.com</t>
   </si>
   <si>
@@ -691,9 +604,6 @@
   </si>
   <si>
     <t>GTH</t>
-  </si>
-  <si>
-    <t>SIGE</t>
   </si>
 </sst>
 </file>
@@ -774,13 +684,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -800,8 +704,8 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Hoja 1-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -813,20 +717,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A2:F80" headerRowCount="0">
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="Hoja 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1030,10 +920,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1048,22 +938,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1071,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1091,7 +981,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -1111,7 +1001,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -1130,8 +1020,8 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>217</v>
+      <c r="B5" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -1151,7 +1041,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -1171,7 +1061,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>16</v>
@@ -1191,7 +1081,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -1211,7 +1101,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
@@ -1231,7 +1121,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>25</v>
@@ -1251,7 +1141,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>28</v>
@@ -1271,7 +1161,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
@@ -1291,7 +1181,7 @@
         <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>34</v>
@@ -1311,7 +1201,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>37</v>
@@ -1331,7 +1221,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>40</v>
@@ -1351,7 +1241,7 @@
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>43</v>
@@ -1371,7 +1261,7 @@
         <v>45</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>46</v>
@@ -1391,7 +1281,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>49</v>
@@ -1411,7 +1301,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>52</v>
@@ -1427,103 +1317,103 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="3">
-        <v>75800004</v>
-      </c>
-      <c r="F20" s="3">
-        <v>971729617</v>
+      <c r="E20" s="4">
+        <v>77903423</v>
+      </c>
+      <c r="F20" s="4">
+        <v>959057558</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="4">
-        <v>70002787</v>
-      </c>
-      <c r="F21" s="4">
-        <v>997001112</v>
+      <c r="E21" s="3">
+        <v>75271965</v>
+      </c>
+      <c r="F21" s="3">
+        <v>921554561</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="3">
-        <v>70271399</v>
-      </c>
-      <c r="F22" s="3">
-        <v>938742086</v>
+      <c r="E22" s="4">
+        <v>71515569</v>
+      </c>
+      <c r="F22" s="4">
+        <v>930287176</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="4">
-        <v>77903423</v>
-      </c>
-      <c r="F23" s="4">
-        <v>959057558</v>
+      <c r="E23" s="3">
+        <v>75867672</v>
+      </c>
+      <c r="F23" s="3">
+        <v>925991081</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="3">
-        <v>75271965</v>
-      </c>
-      <c r="F24" s="3">
-        <v>921554561</v>
+      <c r="E24" s="4">
+        <v>71135621</v>
+      </c>
+      <c r="F24" s="4">
+        <v>962557528</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1531,7 +1421,7 @@
         <v>69</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>70</v>
@@ -1540,10 +1430,10 @@
         <v>71</v>
       </c>
       <c r="E25" s="4">
-        <v>71515569</v>
+        <v>73205899</v>
       </c>
       <c r="F25" s="4">
-        <v>930287176</v>
+        <v>937595709</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1551,7 +1441,7 @@
         <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>73</v>
@@ -1560,10 +1450,10 @@
         <v>74</v>
       </c>
       <c r="E26" s="3">
-        <v>75867672</v>
+        <v>76802354</v>
       </c>
       <c r="F26" s="3">
-        <v>925991081</v>
+        <v>954770675</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1571,7 +1461,7 @@
         <v>75</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>76</v>
@@ -1580,10 +1470,10 @@
         <v>77</v>
       </c>
       <c r="E27" s="4">
-        <v>71135621</v>
+        <v>70572104</v>
       </c>
       <c r="F27" s="4">
-        <v>962557528</v>
+        <v>946870870</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1591,7 +1481,7 @@
         <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>79</v>
@@ -1600,10 +1490,10 @@
         <v>80</v>
       </c>
       <c r="E28" s="3">
-        <v>78017279</v>
+        <v>77351740</v>
       </c>
       <c r="F28" s="3">
-        <v>944278250</v>
+        <v>934342653</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1611,7 +1501,7 @@
         <v>81</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>82</v>
@@ -1620,10 +1510,10 @@
         <v>83</v>
       </c>
       <c r="E29" s="4">
-        <v>72937166</v>
+        <v>75376082</v>
       </c>
       <c r="F29" s="4">
-        <v>981547764</v>
+        <v>936789319</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1631,7 +1521,7 @@
         <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>85</v>
@@ -1640,10 +1530,10 @@
         <v>86</v>
       </c>
       <c r="E30" s="3">
-        <v>70785093</v>
+        <v>60281667</v>
       </c>
       <c r="F30" s="3">
-        <v>938638626</v>
+        <v>912354876</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1651,7 +1541,7 @@
         <v>87</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>88</v>
@@ -1660,10 +1550,10 @@
         <v>89</v>
       </c>
       <c r="E31" s="4">
-        <v>76979368</v>
+        <v>60452764</v>
       </c>
       <c r="F31" s="4">
-        <v>988495943</v>
+        <v>994220839</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1671,7 +1561,7 @@
         <v>90</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>222</v>
+        <v>189</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>91</v>
@@ -1680,10 +1570,10 @@
         <v>92</v>
       </c>
       <c r="E32" s="3">
-        <v>71707370</v>
+        <v>72805119</v>
       </c>
       <c r="F32" s="3">
-        <v>903331889</v>
+        <v>952856050</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1691,7 +1581,7 @@
         <v>93</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>94</v>
@@ -1700,10 +1590,10 @@
         <v>95</v>
       </c>
       <c r="E33" s="4">
-        <v>73205899</v>
+        <v>73538626</v>
       </c>
       <c r="F33" s="4">
-        <v>937595709</v>
+        <v>946722167</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1711,7 +1601,7 @@
         <v>96</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>97</v>
@@ -1720,450 +1610,450 @@
         <v>98</v>
       </c>
       <c r="E34" s="3">
-        <v>76802354</v>
+        <v>71590005</v>
       </c>
       <c r="F34" s="3">
-        <v>954770675</v>
+        <v>990641082</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="4">
-        <v>70572104</v>
-      </c>
-      <c r="F35" s="4">
-        <v>946870870</v>
+      <c r="E35" s="3">
+        <v>71242641</v>
+      </c>
+      <c r="F35" s="3">
+        <v>997237601</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E36" s="3">
-        <v>77351740</v>
-      </c>
-      <c r="F36" s="3">
-        <v>934342653</v>
+      <c r="E36" s="4">
+        <v>70710112</v>
+      </c>
+      <c r="F36" s="4">
+        <v>927977150</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="B37" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E37" s="4">
-        <v>75376082</v>
-      </c>
-      <c r="F37" s="4">
-        <v>936789319</v>
+      <c r="E37" s="3">
+        <v>72476661</v>
+      </c>
+      <c r="F37" s="3">
+        <v>902055267</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E38" s="3">
-        <v>60281667</v>
-      </c>
-      <c r="F38" s="3">
-        <v>912354876</v>
+      <c r="E38" s="4">
+        <v>72917592</v>
+      </c>
+      <c r="F38" s="4">
+        <v>949706787</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E39" s="4">
-        <v>60452764</v>
-      </c>
-      <c r="F39" s="4">
-        <v>994220839</v>
+      <c r="E39" s="3">
+        <v>60593243</v>
+      </c>
+      <c r="F39" s="3">
+        <v>964893379</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B40" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E40" s="3">
-        <v>72805119</v>
-      </c>
-      <c r="F40" s="3">
-        <v>952856050</v>
+      <c r="E40" s="4">
+        <v>60799983</v>
+      </c>
+      <c r="F40" s="4">
+        <v>941768380</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B41" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="4">
-        <v>73538626</v>
-      </c>
-      <c r="F41" s="4">
-        <v>946722167</v>
+      <c r="E41" s="3">
+        <v>70672154</v>
+      </c>
+      <c r="F41" s="3">
+        <v>952629197</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E42" s="3">
-        <v>71590005</v>
-      </c>
-      <c r="F42" s="3">
-        <v>990641082</v>
+      <c r="E42" s="4">
+        <v>73817362</v>
+      </c>
+      <c r="F42" s="4">
+        <v>986643843</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="B43" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E43" s="4">
-        <v>74041150</v>
-      </c>
-      <c r="F43" s="4">
-        <v>945431863</v>
+      <c r="E43" s="3">
+        <v>71274613</v>
+      </c>
+      <c r="F43" s="3">
+        <v>915340183</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B44" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E44" s="3">
-        <v>71242641</v>
-      </c>
-      <c r="F44" s="3">
-        <v>997237601</v>
+      <c r="E44" s="4">
+        <v>71535024</v>
+      </c>
+      <c r="F44" s="4">
+        <v>941832113</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="B45" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E45" s="4">
-        <v>70710112</v>
-      </c>
-      <c r="F45" s="4">
-        <v>927977150</v>
+      <c r="E45" s="3">
+        <v>70511638</v>
+      </c>
+      <c r="F45" s="3">
+        <v>944758194</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E46" s="3">
-        <v>72476661</v>
-      </c>
-      <c r="F46" s="3">
-        <v>902055267</v>
+      <c r="E46" s="4">
+        <v>77673102</v>
+      </c>
+      <c r="F46" s="4">
+        <v>959315773</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="B47" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E47" s="4">
-        <v>72917592</v>
-      </c>
-      <c r="F47" s="4">
-        <v>949706787</v>
+      <c r="E47" s="3">
+        <v>73880963</v>
+      </c>
+      <c r="F47" s="3">
+        <v>932052360</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="B48" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E48" s="3">
-        <v>60593243</v>
-      </c>
-      <c r="F48" s="3">
-        <v>964893379</v>
+      <c r="E48" s="4">
+        <v>60878258</v>
+      </c>
+      <c r="F48" s="4">
+        <v>945509601</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="B49" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E49" s="4">
-        <v>60799983</v>
-      </c>
-      <c r="F49" s="4">
-        <v>941768380</v>
+      <c r="E49" s="3">
+        <v>72456671</v>
+      </c>
+      <c r="F49" s="3">
+        <v>986760857</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="B50" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E50" s="3">
-        <v>70672154</v>
-      </c>
-      <c r="F50" s="3">
-        <v>952629197</v>
+      <c r="E50" s="4">
+        <v>72549352</v>
+      </c>
+      <c r="F50" s="4">
+        <v>919035414</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B51" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E51" s="4">
-        <v>73817362</v>
-      </c>
-      <c r="F51" s="4">
-        <v>986643843</v>
+      <c r="E51" s="3">
+        <v>75533094</v>
+      </c>
+      <c r="F51" s="3">
+        <v>937542434</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B52" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E52" s="3">
-        <v>71274613</v>
-      </c>
-      <c r="F52" s="3">
-        <v>915340183</v>
+      <c r="E52" s="4">
+        <v>60687050</v>
+      </c>
+      <c r="F52" s="4">
+        <v>979157226</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="B53" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E53" s="4">
-        <v>71535024</v>
-      </c>
-      <c r="F53" s="4">
-        <v>941832113</v>
+      <c r="E53" s="3">
+        <v>70703550</v>
+      </c>
+      <c r="F53" s="3">
+        <v>904714632</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B54" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E54" s="3">
-        <v>70511638</v>
-      </c>
-      <c r="F54" s="3">
-        <v>944758194</v>
+      <c r="E54" s="4">
+        <v>60778133</v>
+      </c>
+      <c r="F54" s="4">
+        <v>931450572</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="B55" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E55" s="4">
-        <v>77673102</v>
-      </c>
-      <c r="F55" s="4">
-        <v>959315773</v>
+      <c r="E55" s="3">
+        <v>71005175</v>
+      </c>
+      <c r="F55" s="3">
+        <v>903174167</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="B56" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E56" s="3">
-        <v>73880963</v>
-      </c>
-      <c r="F56" s="3">
-        <v>932052360</v>
+      <c r="E56" s="4">
+        <v>61849038</v>
+      </c>
+      <c r="F56" s="4">
+        <v>954609485</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2171,7 +2061,7 @@
         <v>165</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>166</v>
@@ -2180,10 +2070,10 @@
         <v>167</v>
       </c>
       <c r="E57" s="4">
-        <v>60878258</v>
+        <v>61220475</v>
       </c>
       <c r="F57" s="4">
-        <v>945509601</v>
+        <v>902219499</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2191,7 +2081,7 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>169</v>
@@ -2200,10 +2090,10 @@
         <v>170</v>
       </c>
       <c r="E58" s="3">
-        <v>72456671</v>
+        <v>70711971</v>
       </c>
       <c r="F58" s="3">
-        <v>986760857</v>
+        <v>984591885</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2211,7 +2101,7 @@
         <v>171</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>172</v>
@@ -2220,10 +2110,10 @@
         <v>173</v>
       </c>
       <c r="E59" s="4">
-        <v>72549352</v>
+        <v>72709700</v>
       </c>
       <c r="F59" s="4">
-        <v>919035414</v>
+        <v>996230583</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2231,7 +2121,7 @@
         <v>174</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>175</v>
@@ -2240,416 +2130,194 @@
         <v>176</v>
       </c>
       <c r="E60" s="3">
-        <v>75533094</v>
+        <v>74417161</v>
       </c>
       <c r="F60" s="3">
-        <v>937542434</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+        <v>913893025</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="B61" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E61" s="4">
-        <v>60687050</v>
-      </c>
-      <c r="F61" s="4">
-        <v>979157226</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E62" s="3">
-        <v>70703550</v>
-      </c>
-      <c r="F62" s="3">
-        <v>904714632</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E63" s="4">
-        <v>60778133</v>
-      </c>
-      <c r="F63" s="4">
-        <v>931450572</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="E61" s="3">
+        <v>77568641</v>
+      </c>
+      <c r="F61" s="3">
+        <v>926698691</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="C62" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E62" s="4">
+        <v>61220475</v>
+      </c>
+      <c r="F62" s="4">
+        <v>902219499</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E63" s="3">
+        <v>70711971</v>
+      </c>
+      <c r="F63" s="3">
+        <v>984591885</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E64" s="4">
+        <v>72709700</v>
+      </c>
+      <c r="F64" s="4">
+        <v>996230583</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E65" s="3">
+        <v>74417161</v>
+      </c>
+      <c r="F65" s="3">
+        <v>913893025</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="3">
-        <v>71005175</v>
-      </c>
-      <c r="F64" s="3">
-        <v>903174167</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E66" s="6">
+        <v>77673102</v>
+      </c>
+      <c r="F66" s="6">
+        <v>959315773</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E65" s="4">
-        <v>61849038</v>
-      </c>
-      <c r="F65" s="4">
-        <v>954609485</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E66" s="3">
-        <v>72511722</v>
-      </c>
-      <c r="F66" s="3">
-        <v>925060575</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E67" s="4">
-        <v>61220475</v>
-      </c>
-      <c r="F67" s="4">
-        <v>902219499</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E68" s="3">
-        <v>70711971</v>
-      </c>
-      <c r="F68" s="3">
-        <v>984591885</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E69" s="4">
-        <v>72709700</v>
-      </c>
-      <c r="F69" s="4">
-        <v>996230583</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E70" s="3">
-        <v>74417161</v>
-      </c>
-      <c r="F70" s="3">
-        <v>913893025</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E71" s="4">
-        <v>76979368</v>
-      </c>
-      <c r="F71" s="4">
-        <v>988495943</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E72" s="3">
-        <v>77568641</v>
-      </c>
-      <c r="F72" s="3">
-        <v>926698691</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E73" s="4">
-        <v>61220475</v>
-      </c>
-      <c r="F73" s="4">
-        <v>902219499</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E74" s="3">
-        <v>70711971</v>
-      </c>
-      <c r="F74" s="3">
-        <v>984591885</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E75" s="4">
-        <v>72709700</v>
-      </c>
-      <c r="F75" s="4">
-        <v>996230583</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E76" s="3">
-        <v>74417161</v>
-      </c>
-      <c r="F76" s="3">
-        <v>913893025</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E77" s="6">
-        <v>77673102</v>
-      </c>
-      <c r="F77" s="6">
-        <v>959315773</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E78" s="8">
+      <c r="C67" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E67" s="8">
         <v>73880963</v>
       </c>
-      <c r="F78" s="8">
+      <c r="F67" s="8">
         <v>932052360</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E79" s="6">
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E68" s="6">
         <v>60878258</v>
       </c>
-      <c r="F79" s="6">
+      <c r="F68" s="6">
         <v>945509601</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E80" s="8">
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E69" s="8">
         <v>72456671</v>
       </c>
-      <c r="F80" s="8">
+      <c r="F69" s="8">
         <v>986760857</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix(backend): Arreglado un problema donde fallaba la importación de áreas debido a que se utilizaban ids incorrectos. Ahora las áreas permiten configurar sus siglas. (#29)
</commit_message>
<xml_diff>
--- a/tests/TestFiles/prueba_padron.xlsx
+++ b/tests/TestFiles/prueba_padron.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roberto\Documents\proyectos\votacion-incubunt\tests\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4201399-3EB5-42B0-B84B-62A27B15B6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A711D-501E-44B2-9FDE-C2214F6433B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="192">
   <si>
     <t>diegoagreda51@gmail.com</t>
   </si>
@@ -189,33 +192,6 @@
     <t xml:space="preserve">Chávez Villanueva </t>
   </si>
   <si>
-    <t>echevarriapoemape@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">María De Los Ángeles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Echevarría Poémape </t>
-  </si>
-  <si>
-    <t>ya76larcat@gmail.com</t>
-  </si>
-  <si>
-    <t>Yamille del Pilar</t>
-  </si>
-  <si>
-    <t>Catacora Pinco</t>
-  </si>
-  <si>
-    <t>mellascon29@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mell Julia Kristell </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ascón Aranda </t>
-  </si>
-  <si>
     <t>lrosasp@unitru.edu.pe</t>
   </si>
   <si>
@@ -261,51 +237,6 @@
     <t>Acuña Cisneros</t>
   </si>
   <si>
-    <t>cerquinclaudia669@gmail.com</t>
-  </si>
-  <si>
-    <t>Claudia Yanela</t>
-  </si>
-  <si>
-    <t>Cerquín Alcántara</t>
-  </si>
-  <si>
-    <t>dlazaro@unitru.edu.pe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diana Carolina </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lázaro Solano </t>
-  </si>
-  <si>
-    <t>maria11.07.mfhs@gmail.com</t>
-  </si>
-  <si>
-    <t>Maria Fernanda</t>
-  </si>
-  <si>
-    <t>Holguin Solorzano</t>
-  </si>
-  <si>
-    <t>aurora_merlo@hotmail.com</t>
-  </si>
-  <si>
-    <t>Aurora Nicole</t>
-  </si>
-  <si>
-    <t>Merlo López</t>
-  </si>
-  <si>
-    <t>jcarlosquerebalu@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segundo Jeampier </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carlos Querebalú </t>
-  </si>
-  <si>
     <t>cbarretob@unitru.edu.pe</t>
   </si>
   <si>
@@ -396,15 +327,6 @@
     <t>Correa Urdániga</t>
   </si>
   <si>
-    <t>benitescasanovac@gmail.com</t>
-  </si>
-  <si>
-    <t>Chris Alexandra</t>
-  </si>
-  <si>
-    <t>Benites Casanova</t>
-  </si>
-  <si>
     <t>yasumi.2002.octubre@gmail.com</t>
   </si>
   <si>
@@ -603,15 +525,6 @@
     <t>Vizconde Julca</t>
   </si>
   <si>
-    <t>cristianparimango@gmail.com</t>
-  </si>
-  <si>
-    <t>Cristian Martín</t>
-  </si>
-  <si>
-    <t>Parimango Quispe</t>
-  </si>
-  <si>
     <t>e6666278@gmail.com</t>
   </si>
   <si>
@@ -691,9 +604,6 @@
   </si>
   <si>
     <t>GTH</t>
-  </si>
-  <si>
-    <t>SIGE</t>
   </si>
 </sst>
 </file>
@@ -774,13 +684,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -800,8 +704,8 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Hoja 1-style" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -813,20 +717,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A2:F80" headerRowCount="0">
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="Hoja 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1030,10 +920,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1048,22 +938,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>212</v>
+        <v>182</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>213</v>
+        <v>183</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>214</v>
+        <v>184</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1071,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -1091,7 +981,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -1111,7 +1001,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -1130,8 +1020,8 @@
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>217</v>
+      <c r="B5" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>10</v>
@@ -1151,7 +1041,7 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>218</v>
+        <v>188</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
@@ -1171,7 +1061,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>16</v>
@@ -1191,7 +1081,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>19</v>
@@ -1211,7 +1101,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>22</v>
@@ -1231,7 +1121,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>25</v>
@@ -1251,7 +1141,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>217</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>28</v>
@@ -1271,7 +1161,7 @@
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
@@ -1291,7 +1181,7 @@
         <v>33</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>216</v>
+        <v>186</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>34</v>
@@ -1311,7 +1201,7 @@
         <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>37</v>
@@ -1331,7 +1221,7 @@
         <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>219</v>
+        <v>189</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>40</v>
@@ -1351,7 +1241,7 @@
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>43</v>
@@ -1371,7 +1261,7 @@
         <v>45</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>46</v>
@@ -1391,7 +1281,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>221</v>
+        <v>191</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>49</v>
@@ -1411,7 +1301,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>52</v>
@@ -1427,103 +1317,103 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="B20" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="3">
-        <v>75800004</v>
-      </c>
-      <c r="F20" s="3">
-        <v>971729617</v>
+      <c r="E20" s="4">
+        <v>77903423</v>
+      </c>
+      <c r="F20" s="4">
+        <v>959057558</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="4">
-        <v>70002787</v>
-      </c>
-      <c r="F21" s="4">
-        <v>997001112</v>
+      <c r="E21" s="3">
+        <v>75271965</v>
+      </c>
+      <c r="F21" s="3">
+        <v>921554561</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="3">
-        <v>70271399</v>
-      </c>
-      <c r="F22" s="3">
-        <v>938742086</v>
+      <c r="E22" s="4">
+        <v>71515569</v>
+      </c>
+      <c r="F22" s="4">
+        <v>930287176</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="4">
-        <v>77903423</v>
-      </c>
-      <c r="F23" s="4">
-        <v>959057558</v>
+      <c r="E23" s="3">
+        <v>75867672</v>
+      </c>
+      <c r="F23" s="3">
+        <v>925991081</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="3">
-        <v>75271965</v>
-      </c>
-      <c r="F24" s="3">
-        <v>921554561</v>
+      <c r="E24" s="4">
+        <v>71135621</v>
+      </c>
+      <c r="F24" s="4">
+        <v>962557528</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1531,7 +1421,7 @@
         <v>69</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>70</v>
@@ -1540,10 +1430,10 @@
         <v>71</v>
       </c>
       <c r="E25" s="4">
-        <v>71515569</v>
+        <v>73205899</v>
       </c>
       <c r="F25" s="4">
-        <v>930287176</v>
+        <v>937595709</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1551,7 +1441,7 @@
         <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>73</v>
@@ -1560,10 +1450,10 @@
         <v>74</v>
       </c>
       <c r="E26" s="3">
-        <v>75867672</v>
+        <v>76802354</v>
       </c>
       <c r="F26" s="3">
-        <v>925991081</v>
+        <v>954770675</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1571,7 +1461,7 @@
         <v>75</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>76</v>
@@ -1580,10 +1470,10 @@
         <v>77</v>
       </c>
       <c r="E27" s="4">
-        <v>71135621</v>
+        <v>70572104</v>
       </c>
       <c r="F27" s="4">
-        <v>962557528</v>
+        <v>946870870</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1591,7 +1481,7 @@
         <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>79</v>
@@ -1600,10 +1490,10 @@
         <v>80</v>
       </c>
       <c r="E28" s="3">
-        <v>78017279</v>
+        <v>77351740</v>
       </c>
       <c r="F28" s="3">
-        <v>944278250</v>
+        <v>934342653</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1611,7 +1501,7 @@
         <v>81</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>82</v>
@@ -1620,10 +1510,10 @@
         <v>83</v>
       </c>
       <c r="E29" s="4">
-        <v>72937166</v>
+        <v>75376082</v>
       </c>
       <c r="F29" s="4">
-        <v>981547764</v>
+        <v>936789319</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1631,7 +1521,7 @@
         <v>84</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>85</v>
@@ -1640,10 +1530,10 @@
         <v>86</v>
       </c>
       <c r="E30" s="3">
-        <v>70785093</v>
+        <v>60281667</v>
       </c>
       <c r="F30" s="3">
-        <v>938638626</v>
+        <v>912354876</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1651,7 +1541,7 @@
         <v>87</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>88</v>
@@ -1660,10 +1550,10 @@
         <v>89</v>
       </c>
       <c r="E31" s="4">
-        <v>76979368</v>
+        <v>60452764</v>
       </c>
       <c r="F31" s="4">
-        <v>988495943</v>
+        <v>994220839</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1671,7 +1561,7 @@
         <v>90</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>222</v>
+        <v>189</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>91</v>
@@ -1680,10 +1570,10 @@
         <v>92</v>
       </c>
       <c r="E32" s="3">
-        <v>71707370</v>
+        <v>72805119</v>
       </c>
       <c r="F32" s="3">
-        <v>903331889</v>
+        <v>952856050</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1691,7 +1581,7 @@
         <v>93</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>94</v>
@@ -1700,10 +1590,10 @@
         <v>95</v>
       </c>
       <c r="E33" s="4">
-        <v>73205899</v>
+        <v>73538626</v>
       </c>
       <c r="F33" s="4">
-        <v>937595709</v>
+        <v>946722167</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -1711,7 +1601,7 @@
         <v>96</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>97</v>
@@ -1720,450 +1610,450 @@
         <v>98</v>
       </c>
       <c r="E34" s="3">
-        <v>76802354</v>
+        <v>71590005</v>
       </c>
       <c r="F34" s="3">
-        <v>954770675</v>
+        <v>990641082</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B35" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="4">
-        <v>70572104</v>
-      </c>
-      <c r="F35" s="4">
-        <v>946870870</v>
+      <c r="E35" s="3">
+        <v>71242641</v>
+      </c>
+      <c r="F35" s="3">
+        <v>997237601</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E36" s="3">
-        <v>77351740</v>
-      </c>
-      <c r="F36" s="3">
-        <v>934342653</v>
+      <c r="E36" s="4">
+        <v>70710112</v>
+      </c>
+      <c r="F36" s="4">
+        <v>927977150</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="B37" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E37" s="4">
-        <v>75376082</v>
-      </c>
-      <c r="F37" s="4">
-        <v>936789319</v>
+      <c r="E37" s="3">
+        <v>72476661</v>
+      </c>
+      <c r="F37" s="3">
+        <v>902055267</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E38" s="3">
-        <v>60281667</v>
-      </c>
-      <c r="F38" s="3">
-        <v>912354876</v>
+      <c r="E38" s="4">
+        <v>72917592</v>
+      </c>
+      <c r="F38" s="4">
+        <v>949706787</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E39" s="4">
-        <v>60452764</v>
-      </c>
-      <c r="F39" s="4">
-        <v>994220839</v>
+      <c r="E39" s="3">
+        <v>60593243</v>
+      </c>
+      <c r="F39" s="3">
+        <v>964893379</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C40" s="1" t="s">
+      <c r="B40" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E40" s="3">
-        <v>72805119</v>
-      </c>
-      <c r="F40" s="3">
-        <v>952856050</v>
+      <c r="E40" s="4">
+        <v>60799983</v>
+      </c>
+      <c r="F40" s="4">
+        <v>941768380</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B41" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E41" s="4">
-        <v>73538626</v>
-      </c>
-      <c r="F41" s="4">
-        <v>946722167</v>
+      <c r="E41" s="3">
+        <v>70672154</v>
+      </c>
+      <c r="F41" s="3">
+        <v>952629197</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E42" s="3">
-        <v>71590005</v>
-      </c>
-      <c r="F42" s="3">
-        <v>990641082</v>
+      <c r="E42" s="4">
+        <v>73817362</v>
+      </c>
+      <c r="F42" s="4">
+        <v>986643843</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="B43" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E43" s="4">
-        <v>74041150</v>
-      </c>
-      <c r="F43" s="4">
-        <v>945431863</v>
+      <c r="E43" s="3">
+        <v>71274613</v>
+      </c>
+      <c r="F43" s="3">
+        <v>915340183</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C44" s="1" t="s">
+      <c r="B44" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E44" s="3">
-        <v>71242641</v>
-      </c>
-      <c r="F44" s="3">
-        <v>997237601</v>
+      <c r="E44" s="4">
+        <v>71535024</v>
+      </c>
+      <c r="F44" s="4">
+        <v>941832113</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="B45" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E45" s="4">
-        <v>70710112</v>
-      </c>
-      <c r="F45" s="4">
-        <v>927977150</v>
+      <c r="E45" s="3">
+        <v>70511638</v>
+      </c>
+      <c r="F45" s="3">
+        <v>944758194</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E46" s="3">
-        <v>72476661</v>
-      </c>
-      <c r="F46" s="3">
-        <v>902055267</v>
+      <c r="E46" s="4">
+        <v>77673102</v>
+      </c>
+      <c r="F46" s="4">
+        <v>959315773</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C47" s="2" t="s">
+      <c r="B47" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E47" s="4">
-        <v>72917592</v>
-      </c>
-      <c r="F47" s="4">
-        <v>949706787</v>
+      <c r="E47" s="3">
+        <v>73880963</v>
+      </c>
+      <c r="F47" s="3">
+        <v>932052360</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C48" s="1" t="s">
+      <c r="B48" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E48" s="3">
-        <v>60593243</v>
-      </c>
-      <c r="F48" s="3">
-        <v>964893379</v>
+      <c r="E48" s="4">
+        <v>60878258</v>
+      </c>
+      <c r="F48" s="4">
+        <v>945509601</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="B49" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D49" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E49" s="4">
-        <v>60799983</v>
-      </c>
-      <c r="F49" s="4">
-        <v>941768380</v>
+      <c r="E49" s="3">
+        <v>72456671</v>
+      </c>
+      <c r="F49" s="3">
+        <v>986760857</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C50" s="1" t="s">
+      <c r="B50" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E50" s="3">
-        <v>70672154</v>
-      </c>
-      <c r="F50" s="3">
-        <v>952629197</v>
+      <c r="E50" s="4">
+        <v>72549352</v>
+      </c>
+      <c r="F50" s="4">
+        <v>919035414</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B51" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E51" s="4">
-        <v>73817362</v>
-      </c>
-      <c r="F51" s="4">
-        <v>986643843</v>
+      <c r="E51" s="3">
+        <v>75533094</v>
+      </c>
+      <c r="F51" s="3">
+        <v>937542434</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C52" s="1" t="s">
+      <c r="B52" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E52" s="3">
-        <v>71274613</v>
-      </c>
-      <c r="F52" s="3">
-        <v>915340183</v>
+      <c r="E52" s="4">
+        <v>60687050</v>
+      </c>
+      <c r="F52" s="4">
+        <v>979157226</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="B53" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D53" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E53" s="4">
-        <v>71535024</v>
-      </c>
-      <c r="F53" s="4">
-        <v>941832113</v>
+      <c r="E53" s="3">
+        <v>70703550</v>
+      </c>
+      <c r="F53" s="3">
+        <v>904714632</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B54" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E54" s="3">
-        <v>70511638</v>
-      </c>
-      <c r="F54" s="3">
-        <v>944758194</v>
+      <c r="E54" s="4">
+        <v>60778133</v>
+      </c>
+      <c r="F54" s="4">
+        <v>931450572</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="B55" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E55" s="4">
-        <v>77673102</v>
-      </c>
-      <c r="F55" s="4">
-        <v>959315773</v>
+      <c r="E55" s="3">
+        <v>71005175</v>
+      </c>
+      <c r="F55" s="3">
+        <v>903174167</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="B56" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E56" s="3">
-        <v>73880963</v>
-      </c>
-      <c r="F56" s="3">
-        <v>932052360</v>
+      <c r="E56" s="4">
+        <v>61849038</v>
+      </c>
+      <c r="F56" s="4">
+        <v>954609485</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2171,7 +2061,7 @@
         <v>165</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>166</v>
@@ -2180,10 +2070,10 @@
         <v>167</v>
       </c>
       <c r="E57" s="4">
-        <v>60878258</v>
+        <v>61220475</v>
       </c>
       <c r="F57" s="4">
-        <v>945509601</v>
+        <v>902219499</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2191,7 +2081,7 @@
         <v>168</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>220</v>
+        <v>187</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>169</v>
@@ -2200,10 +2090,10 @@
         <v>170</v>
       </c>
       <c r="E58" s="3">
-        <v>72456671</v>
+        <v>70711971</v>
       </c>
       <c r="F58" s="3">
-        <v>986760857</v>
+        <v>984591885</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2211,7 +2101,7 @@
         <v>171</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>172</v>
@@ -2220,10 +2110,10 @@
         <v>173</v>
       </c>
       <c r="E59" s="4">
-        <v>72549352</v>
+        <v>72709700</v>
       </c>
       <c r="F59" s="4">
-        <v>919035414</v>
+        <v>996230583</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -2231,7 +2121,7 @@
         <v>174</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>175</v>
@@ -2240,416 +2130,194 @@
         <v>176</v>
       </c>
       <c r="E60" s="3">
-        <v>75533094</v>
+        <v>74417161</v>
       </c>
       <c r="F60" s="3">
-        <v>937542434</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
+        <v>913893025</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="B61" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="D61" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E61" s="4">
-        <v>60687050</v>
-      </c>
-      <c r="F61" s="4">
-        <v>979157226</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E62" s="3">
-        <v>70703550</v>
-      </c>
-      <c r="F62" s="3">
-        <v>904714632</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E63" s="4">
-        <v>60778133</v>
-      </c>
-      <c r="F63" s="4">
-        <v>931450572</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="E61" s="3">
+        <v>77568641</v>
+      </c>
+      <c r="F61" s="3">
+        <v>926698691</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="C62" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E62" s="4">
+        <v>61220475</v>
+      </c>
+      <c r="F62" s="4">
+        <v>902219499</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E63" s="3">
+        <v>70711971</v>
+      </c>
+      <c r="F63" s="3">
+        <v>984591885</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E64" s="4">
+        <v>72709700</v>
+      </c>
+      <c r="F64" s="4">
+        <v>996230583</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E65" s="3">
+        <v>74417161</v>
+      </c>
+      <c r="F65" s="3">
+        <v>913893025</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="E64" s="3">
-        <v>71005175</v>
-      </c>
-      <c r="F64" s="3">
-        <v>903174167</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C65" s="2" t="s">
+      <c r="C66" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E66" s="6">
+        <v>77673102</v>
+      </c>
+      <c r="F66" s="6">
+        <v>959315773</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E65" s="4">
-        <v>61849038</v>
-      </c>
-      <c r="F65" s="4">
-        <v>954609485</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E66" s="3">
-        <v>72511722</v>
-      </c>
-      <c r="F66" s="3">
-        <v>925060575</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E67" s="4">
-        <v>61220475</v>
-      </c>
-      <c r="F67" s="4">
-        <v>902219499</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E68" s="3">
-        <v>70711971</v>
-      </c>
-      <c r="F68" s="3">
-        <v>984591885</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E69" s="4">
-        <v>72709700</v>
-      </c>
-      <c r="F69" s="4">
-        <v>996230583</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E70" s="3">
-        <v>74417161</v>
-      </c>
-      <c r="F70" s="3">
-        <v>913893025</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E71" s="4">
-        <v>76979368</v>
-      </c>
-      <c r="F71" s="4">
-        <v>988495943</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="E72" s="3">
-        <v>77568641</v>
-      </c>
-      <c r="F72" s="3">
-        <v>926698691</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="E73" s="4">
-        <v>61220475</v>
-      </c>
-      <c r="F73" s="4">
-        <v>902219499</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E74" s="3">
-        <v>70711971</v>
-      </c>
-      <c r="F74" s="3">
-        <v>984591885</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E75" s="4">
-        <v>72709700</v>
-      </c>
-      <c r="F75" s="4">
-        <v>996230583</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E76" s="3">
-        <v>74417161</v>
-      </c>
-      <c r="F76" s="3">
-        <v>913893025</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="E77" s="6">
-        <v>77673102</v>
-      </c>
-      <c r="F77" s="6">
-        <v>959315773</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="E78" s="8">
+      <c r="C67" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E67" s="8">
         <v>73880963</v>
       </c>
-      <c r="F78" s="8">
+      <c r="F67" s="8">
         <v>932052360</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="E79" s="6">
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E68" s="6">
         <v>60878258</v>
       </c>
-      <c r="F79" s="6">
+      <c r="F68" s="6">
         <v>945509601</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="E80" s="8">
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E69" s="8">
         <v>72456671</v>
       </c>
-      <c r="F80" s="8">
+      <c r="F69" s="8">
         <v>986760857</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>